<commit_message>
Update thesauri map triples
</commit_message>
<xml_diff>
--- a/gallery_buchanan/classification/ThesauriMap.xlsx
+++ b/gallery_buchanan/classification/ThesauriMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baskausj/github/vandycite/gallery_buchanan/classification/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/621eba9d3d6ef5ee/Librarian/UTK MSIS Courses/INSC - ^N^N^N Internship/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2A22FF-B578-A647-9CB6-F609DA02698B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="738" documentId="8_{90E60F8B-E1FA-4101-BF0C-5A4AB88A8312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53955454-9157-45CE-ABDB-26EFA69B495C}"/>
   <bookViews>
-    <workbookView xWindow="9760" yWindow="500" windowWidth="41440" windowHeight="26700" activeTab="2" xr2:uid="{F252BA0C-C792-491B-8974-6FBBF34C2951}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{F252BA0C-C792-491B-8974-6FBBF34C2951}"/>
   </bookViews>
   <sheets>
     <sheet name="AllTermsMap" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="930">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="928">
   <si>
     <t>noun</t>
   </si>
@@ -2434,9 +2434,6 @@
     <t>biblical and artistic theme of the Virgin Mary cradling the dead body of Jesus</t>
   </si>
   <si>
-    <t>Question: should this also have a second classification of sculture or statuette</t>
-  </si>
-  <si>
     <t>handle of an edged weapon</t>
   </si>
   <si>
@@ -2446,18 +2443,9 @@
     <t>The Smithsonian categorizes several of their cong's using the nom:12986 term.</t>
   </si>
   <si>
-    <t>Could broader Nomen term for edged Weapons be used?</t>
-  </si>
-  <si>
     <t>Ceremonial chairs or seats occupied by a monarch, prelate, or other high dignitary, especially on state or other special occasions; usually placed upon a dais and covered with a canopy.</t>
   </si>
   <si>
-    <t>nom:1090, chair $ nom:12986, ceremonial objects</t>
-  </si>
-  <si>
-    <t>I wonder if we used two nomen terms that would help.</t>
-  </si>
-  <si>
     <t>Tsuba (鍔 or 鐔): The tsuba is a hand guard. Plate guards of a Japanese sword that separate the blade from the handle. Typically, tsuba are round or kite- shaped, having a central opening for the tang of the blade and occasionally surrounded by a smaller perforations. They vary in size from about 8 to 15 centimeters, depending on the length of the blade. While tsuba were a functional part of the sword, they also evolved into an art form in their own right around the late 15th century and peaking in the 19th century. Materials can range from iron, brass, and steel to gold and silver, and rare ones of ivory or wood.</t>
   </si>
   <si>
@@ -2506,9 +2494,6 @@
     <t>Translation</t>
   </si>
   <si>
-    <t>http://www.wikidata.org/entity/Q20983128</t>
-  </si>
-  <si>
     <t>S Soba Choka, P has broad match , O cups (drinking vessels)</t>
   </si>
   <si>
@@ -2663,9 +2648,6 @@
   </si>
   <si>
     <t>S sashi, P has broad match, O Clothing Accessories &amp; Components</t>
-  </si>
-  <si>
-    <t>broader match -wikidata records says this is instance of wd:Q1065579, costume accessory /  This could match to aat:300209273, costume accessories, but aat:300423330 is better ecause equivalent to $ nom:2000, clothing accessories &amp; components</t>
   </si>
   <si>
     <t>http://vocab.getty.edu/aat/300423330</t>
@@ -2732,9 +2714,6 @@
     <t>nom:5221, drink serving vessel</t>
   </si>
   <si>
-    <t>No similar term in nomen or appropriate broader match.</t>
-  </si>
-  <si>
     <t>http://www.wikidata.org/entity/Q476968</t>
   </si>
   <si>
@@ -2742,12 +2721,6 @@
   </si>
   <si>
     <t>S krater, P has broad match, O drink serving vessels</t>
-  </si>
-  <si>
-    <t>https://nomenclature.info/nom/12895</t>
-  </si>
-  <si>
-    <t>BT - nom:12895, visual art</t>
   </si>
   <si>
     <t>http://www.wikidata.org/entity/Q223689</t>
@@ -2763,9 +2736,6 @@
     <t>S hilt, P has broad match, O Armament Accessories &amp; Components</t>
   </si>
   <si>
-    <t>S pieta, P has broad match, O visual art</t>
-  </si>
-  <si>
     <t>nom:12986, Ceremonial object  or nom:13120, ritual container</t>
   </si>
   <si>
@@ -2781,9 +2751,6 @@
     <t>https://www.nomenclature.info/nom/4771</t>
   </si>
   <si>
-    <t>S cong, P has broad match, O ritual vessel</t>
-  </si>
-  <si>
     <t>S kylix, P has broad match, O cup</t>
   </si>
   <si>
@@ -2802,12 +2769,6 @@
     <t>S throne, P has broad match, O chair</t>
   </si>
   <si>
-    <t>https://www.nomenclature.info/nom/12986</t>
-  </si>
-  <si>
-    <t>S throne, P has broad match, O ceremonial objects</t>
-  </si>
-  <si>
     <t>Vocab Uris</t>
   </si>
   <si>
@@ -2830,13 +2791,61 @@
   </si>
   <si>
     <t>I think the most generic match is the best we can do here, so I chose the category term: https://nomenclature.info/nom/3176 ; another option would be to analyze the objects to determine if there is a more appropriate specific term in all three vocabularies, but since these objects may not have much context information to begin with, a generic term/class is probably the most appropriate.</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q3087145</t>
+  </si>
+  <si>
+    <t>S pommel, P has broad match, O Armament Accessories &amp; Components</t>
+  </si>
+  <si>
+    <t>Question: should this also have a second classification of sculture or statuette
+Update: discussion with Steve/Chuck; we felt it was best to keep the one to one relationship of one WikiData term to one term each of the other vocabs.</t>
+  </si>
+  <si>
+    <t>Could broader Nomen term for edged Weapons be used?
+Update: decided to stick with the Armament Accessories category</t>
+  </si>
+  <si>
+    <t>S cong, P has broad match, O ritual container</t>
+  </si>
+  <si>
+    <t>I wonder if we used two nomen terms that would help. UPDATE: per discussion with Steve/Chuck; we elt it was best to keep the one to one relationship as per the note for Pieta.</t>
+  </si>
+  <si>
+    <t>Update: BT - nom:12898, vistual work rather than BT - nom:12895, visual arts</t>
+  </si>
+  <si>
+    <t>https://nomenclature.info/nom/12898</t>
+  </si>
+  <si>
+    <t>S pieta, P has broad match, O visual work</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">nom:1090, chair $ </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nom:12986, ceremonial objects</t>
+    </r>
+  </si>
+  <si>
+    <t>broader match -wikidata records says this is instance of wd:Q1065579, costume accessory /  This could match to aat:300209273, costume accessories, but aat:300423330 is better because equivalent to $ nom:2000, clothing accessories &amp; components</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2868,7 +2877,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial Unicode MS"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -2876,8 +2884,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2887,12 +2916,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2924,7 +2947,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2951,8 +2974,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3040,6 +3069,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3345,19 +3378,19 @@
       <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3386,7 +3419,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3412,7 +3445,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3438,7 +3471,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -3464,7 +3497,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -3481,7 +3514,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -3507,7 +3540,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -3533,7 +3566,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -3559,7 +3592,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -3585,7 +3618,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -3611,7 +3644,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -3625,7 +3658,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -3651,7 +3684,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -3677,7 +3710,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -3703,7 +3736,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -3729,7 +3762,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -3755,7 +3788,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -3781,7 +3814,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -3807,7 +3840,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>75</v>
       </c>
@@ -3833,7 +3866,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>79</v>
       </c>
@@ -3859,7 +3892,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -3885,7 +3918,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>89</v>
       </c>
@@ -3911,7 +3944,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>94</v>
       </c>
@@ -3937,7 +3970,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -3957,7 +3990,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -3983,7 +4016,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -4009,7 +4042,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>108</v>
       </c>
@@ -4035,7 +4068,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>113</v>
       </c>
@@ -4061,7 +4094,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>117</v>
       </c>
@@ -4087,7 +4120,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>122</v>
       </c>
@@ -4113,7 +4146,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>126</v>
       </c>
@@ -4139,7 +4172,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>129</v>
       </c>
@@ -4153,7 +4186,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>132</v>
       </c>
@@ -4173,7 +4206,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>135</v>
       </c>
@@ -4193,7 +4226,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>137</v>
       </c>
@@ -4219,7 +4252,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -4245,7 +4278,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>145</v>
       </c>
@@ -4271,7 +4304,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>149</v>
       </c>
@@ -4297,7 +4330,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>153</v>
       </c>
@@ -4323,7 +4356,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>158</v>
       </c>
@@ -4349,7 +4382,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>163</v>
       </c>
@@ -4375,7 +4408,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>167</v>
       </c>
@@ -4401,7 +4434,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>171</v>
       </c>
@@ -4427,7 +4460,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>175</v>
       </c>
@@ -4453,7 +4486,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>179</v>
       </c>
@@ -4479,7 +4512,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>183</v>
       </c>
@@ -4505,7 +4538,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>187</v>
       </c>
@@ -4531,7 +4564,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>191</v>
       </c>
@@ -4551,7 +4584,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>194</v>
       </c>
@@ -4577,7 +4610,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>198</v>
       </c>
@@ -4603,7 +4636,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>202</v>
       </c>
@@ -4629,7 +4662,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>206</v>
       </c>
@@ -4655,7 +4688,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>210</v>
       </c>
@@ -4681,7 +4714,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>214</v>
       </c>
@@ -4707,7 +4740,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>218</v>
       </c>
@@ -4733,7 +4766,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>222</v>
       </c>
@@ -4759,7 +4792,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>226</v>
       </c>
@@ -4779,7 +4812,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>230</v>
       </c>
@@ -4805,7 +4838,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>235</v>
       </c>
@@ -4831,7 +4864,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>240</v>
       </c>
@@ -4857,7 +4890,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>161</v>
       </c>
@@ -4883,7 +4916,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>246</v>
       </c>
@@ -4909,7 +4942,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>250</v>
       </c>
@@ -4935,7 +4968,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>254</v>
       </c>
@@ -4961,7 +4994,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>258</v>
       </c>
@@ -4987,7 +5020,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
         <v>262</v>
       </c>
@@ -5013,7 +5046,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>266</v>
       </c>
@@ -5039,7 +5072,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>270</v>
       </c>
@@ -5065,7 +5098,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>275</v>
       </c>
@@ -5091,7 +5124,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>279</v>
       </c>
@@ -5117,7 +5150,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
         <v>283</v>
       </c>
@@ -5143,7 +5176,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
         <v>287</v>
       </c>
@@ -5157,7 +5190,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8">
       <c r="A73" t="s">
         <v>290</v>
       </c>
@@ -5177,7 +5210,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8">
       <c r="A74" t="s">
         <v>293</v>
       </c>
@@ -5203,7 +5236,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>297</v>
       </c>
@@ -5229,7 +5262,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8">
       <c r="A76" t="s">
         <v>301</v>
       </c>
@@ -5255,7 +5288,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8">
       <c r="A77" t="s">
         <v>305</v>
       </c>
@@ -5281,7 +5314,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
         <v>308</v>
       </c>
@@ -5307,7 +5340,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
         <v>312</v>
       </c>
@@ -5333,7 +5366,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
         <v>316</v>
       </c>
@@ -5359,7 +5392,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8">
       <c r="A81" t="s">
         <v>320</v>
       </c>
@@ -5385,7 +5418,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8">
       <c r="A82" t="s">
         <v>324</v>
       </c>
@@ -5405,7 +5438,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>328</v>
       </c>
@@ -5431,7 +5464,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8">
       <c r="A84" t="s">
         <v>333</v>
       </c>
@@ -5445,7 +5478,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>335</v>
       </c>
@@ -5471,7 +5504,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>340</v>
       </c>
@@ -5497,7 +5530,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
         <v>344</v>
       </c>
@@ -5523,7 +5556,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>348</v>
       </c>
@@ -5549,7 +5582,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
         <v>352</v>
       </c>
@@ -5575,7 +5608,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8">
       <c r="A90" t="s">
         <v>357</v>
       </c>
@@ -5601,7 +5634,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8">
       <c r="A91" t="s">
         <v>361</v>
       </c>
@@ -5627,7 +5660,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8">
       <c r="A92" t="s">
         <v>365</v>
       </c>
@@ -5653,7 +5686,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8">
       <c r="A93" t="s">
         <v>369</v>
       </c>
@@ -5679,7 +5712,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8">
       <c r="A94" t="s">
         <v>373</v>
       </c>
@@ -5705,7 +5738,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8">
       <c r="A95" t="s">
         <v>377</v>
       </c>
@@ -5731,7 +5764,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8">
       <c r="A96" t="s">
         <v>382</v>
       </c>
@@ -5757,7 +5790,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8">
       <c r="A97" t="s">
         <v>386</v>
       </c>
@@ -5783,7 +5816,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8">
       <c r="A98" t="s">
         <v>390</v>
       </c>
@@ -5803,7 +5836,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8">
       <c r="A99" t="s">
         <v>392</v>
       </c>
@@ -5829,7 +5862,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8">
       <c r="A100" t="s">
         <v>396</v>
       </c>
@@ -5855,7 +5888,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8">
       <c r="A101" t="s">
         <v>400</v>
       </c>
@@ -5881,7 +5914,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8">
       <c r="A102" t="s">
         <v>404</v>
       </c>
@@ -5907,7 +5940,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8">
       <c r="A103" t="s">
         <v>409</v>
       </c>
@@ -5933,7 +5966,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8">
       <c r="A104" t="s">
         <v>413</v>
       </c>
@@ -5959,7 +5992,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8">
       <c r="A105" t="s">
         <v>417</v>
       </c>
@@ -5985,7 +6018,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8">
       <c r="A106" t="s">
         <v>421</v>
       </c>
@@ -5999,7 +6032,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8">
       <c r="A107" t="s">
         <v>423</v>
       </c>
@@ -6025,7 +6058,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8">
       <c r="A108" t="s">
         <v>426</v>
       </c>
@@ -6051,7 +6084,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8">
       <c r="A109" t="s">
         <v>430</v>
       </c>
@@ -6077,7 +6110,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8">
       <c r="A110" t="s">
         <v>434</v>
       </c>
@@ -6103,7 +6136,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8">
       <c r="A111" t="s">
         <v>438</v>
       </c>
@@ -6129,7 +6162,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8">
       <c r="A112" t="s">
         <v>442</v>
       </c>
@@ -6155,7 +6188,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8">
       <c r="A113" t="s">
         <v>447</v>
       </c>
@@ -6169,7 +6202,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8">
       <c r="A114" t="s">
         <v>450</v>
       </c>
@@ -6189,7 +6222,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8">
       <c r="A115" t="s">
         <v>454</v>
       </c>
@@ -6215,7 +6248,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8">
       <c r="A116" t="s">
         <v>458</v>
       </c>
@@ -6241,7 +6274,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8">
       <c r="A117" t="s">
         <v>462</v>
       </c>
@@ -6261,7 +6294,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8">
       <c r="A118" t="s">
         <v>465</v>
       </c>
@@ -6287,7 +6320,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8">
       <c r="A119" t="s">
         <v>469</v>
       </c>
@@ -6313,7 +6346,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8">
       <c r="A120" t="s">
         <v>474</v>
       </c>
@@ -6339,7 +6372,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8">
       <c r="A121" t="s">
         <v>478</v>
       </c>
@@ -6359,7 +6392,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8">
       <c r="A122" t="s">
         <v>482</v>
       </c>
@@ -6385,7 +6418,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8">
       <c r="A123" t="s">
         <v>486</v>
       </c>
@@ -6411,7 +6444,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8">
       <c r="A124" t="s">
         <v>490</v>
       </c>
@@ -6437,7 +6470,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8">
       <c r="A125" t="s">
         <v>494</v>
       </c>
@@ -6463,7 +6496,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8">
       <c r="A126" t="s">
         <v>498</v>
       </c>
@@ -6483,7 +6516,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8">
       <c r="A127" t="s">
         <v>502</v>
       </c>
@@ -6509,7 +6542,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8">
       <c r="A128" t="s">
         <v>506</v>
       </c>
@@ -6535,7 +6568,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8">
       <c r="A129" t="s">
         <v>510</v>
       </c>
@@ -6561,7 +6594,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8">
       <c r="A130" t="s">
         <v>514</v>
       </c>
@@ -6587,7 +6620,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8">
       <c r="A131" t="s">
         <v>518</v>
       </c>
@@ -6613,7 +6646,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8">
       <c r="A132" t="s">
         <v>522</v>
       </c>
@@ -6639,7 +6672,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8">
       <c r="A133" t="s">
         <v>526</v>
       </c>
@@ -6665,7 +6698,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8">
       <c r="A134" t="s">
         <v>529</v>
       </c>
@@ -6691,7 +6724,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8">
       <c r="A135" t="s">
         <v>532</v>
       </c>
@@ -6717,7 +6750,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8">
       <c r="A136" t="s">
         <v>536</v>
       </c>
@@ -6743,7 +6776,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8">
       <c r="A137" t="s">
         <v>540</v>
       </c>
@@ -6769,7 +6802,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8">
       <c r="A138" t="s">
         <v>543</v>
       </c>
@@ -6795,7 +6828,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8">
       <c r="A139" t="s">
         <v>547</v>
       </c>
@@ -6821,7 +6854,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8">
       <c r="A140" t="s">
         <v>552</v>
       </c>
@@ -6847,7 +6880,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8">
       <c r="A141" t="s">
         <v>556</v>
       </c>
@@ -6873,7 +6906,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8">
       <c r="A142" t="s">
         <v>560</v>
       </c>
@@ -6893,7 +6926,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8">
       <c r="A143" t="s">
         <v>563</v>
       </c>
@@ -6919,7 +6952,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8">
       <c r="A144" t="s">
         <v>567</v>
       </c>
@@ -6945,7 +6978,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8">
       <c r="A145" t="s">
         <v>571</v>
       </c>
@@ -6971,7 +7004,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8">
       <c r="A146" t="s">
         <v>576</v>
       </c>
@@ -6997,7 +7030,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8">
       <c r="A147" t="s">
         <v>580</v>
       </c>
@@ -7023,7 +7056,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8">
       <c r="A148" t="s">
         <v>584</v>
       </c>
@@ -7049,7 +7082,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8">
       <c r="A149" t="s">
         <v>589</v>
       </c>
@@ -7075,7 +7108,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8">
       <c r="A150" t="s">
         <v>592</v>
       </c>
@@ -7101,7 +7134,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8">
       <c r="A151" t="s">
         <v>596</v>
       </c>
@@ -7127,7 +7160,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:8">
       <c r="A152" t="s">
         <v>600</v>
       </c>
@@ -7153,7 +7186,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8">
       <c r="A153" t="s">
         <v>604</v>
       </c>
@@ -7179,7 +7212,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8">
       <c r="A154" t="s">
         <v>608</v>
       </c>
@@ -7205,7 +7238,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8">
       <c r="A155" t="s">
         <v>612</v>
       </c>
@@ -7231,7 +7264,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8">
       <c r="A156" t="s">
         <v>616</v>
       </c>
@@ -7257,7 +7290,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8">
       <c r="A157" t="s">
         <v>620</v>
       </c>
@@ -7283,7 +7316,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8">
       <c r="A158" t="s">
         <v>624</v>
       </c>
@@ -7309,7 +7342,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8">
       <c r="A159" t="s">
         <v>629</v>
       </c>
@@ -7335,7 +7368,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8">
       <c r="A160" t="s">
         <v>633</v>
       </c>
@@ -7355,7 +7388,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8">
       <c r="A161" t="s">
         <v>636</v>
       </c>
@@ -7381,7 +7414,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8">
       <c r="A162" t="s">
         <v>640</v>
       </c>
@@ -7407,7 +7440,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8">
       <c r="A163" t="s">
         <v>644</v>
       </c>
@@ -7433,7 +7466,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8">
       <c r="A164" t="s">
         <v>648</v>
       </c>
@@ -7459,7 +7492,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8">
       <c r="A165" t="s">
         <v>652</v>
       </c>
@@ -7485,7 +7518,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8">
       <c r="A166" t="s">
         <v>656</v>
       </c>
@@ -7511,7 +7544,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8">
       <c r="A167" t="s">
         <v>660</v>
       </c>
@@ -7537,7 +7570,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8">
       <c r="A168" t="s">
         <v>664</v>
       </c>
@@ -7563,7 +7596,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8">
       <c r="A169" t="s">
         <v>669</v>
       </c>
@@ -7589,7 +7622,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8">
       <c r="A170" t="s">
         <v>673</v>
       </c>
@@ -7615,7 +7648,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8">
       <c r="A171" t="s">
         <v>677</v>
       </c>
@@ -7641,7 +7674,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8">
       <c r="A172" t="s">
         <v>682</v>
       </c>
@@ -7667,7 +7700,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8">
       <c r="A173" t="s">
         <v>686</v>
       </c>
@@ -7693,7 +7726,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8">
       <c r="A174" t="s">
         <v>690</v>
       </c>
@@ -7719,7 +7752,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8">
       <c r="A175" t="s">
         <v>694</v>
       </c>
@@ -7745,7 +7778,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8">
       <c r="A176" t="s">
         <v>698</v>
       </c>
@@ -7771,7 +7804,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8">
       <c r="A177" t="s">
         <v>702</v>
       </c>
@@ -7797,7 +7830,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8">
       <c r="A178" t="s">
         <v>707</v>
       </c>
@@ -7823,7 +7856,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8">
       <c r="A179" t="s">
         <v>711</v>
       </c>
@@ -7849,7 +7882,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8">
       <c r="A180" t="s">
         <v>715</v>
       </c>
@@ -7875,7 +7908,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8">
       <c r="A181" t="s">
         <v>719</v>
       </c>
@@ -7901,7 +7934,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8">
       <c r="A182" t="s">
         <v>724</v>
       </c>
@@ -7927,7 +7960,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8">
       <c r="A183" t="s">
         <v>728</v>
       </c>
@@ -7953,7 +7986,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8">
       <c r="A184" t="s">
         <v>732</v>
       </c>
@@ -7973,7 +8006,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8">
       <c r="A185" t="s">
         <v>736</v>
       </c>
@@ -7999,7 +8032,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8">
       <c r="A186" t="s">
         <v>740</v>
       </c>
@@ -8025,7 +8058,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8">
       <c r="A187" t="s">
         <v>744</v>
       </c>
@@ -8045,7 +8078,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8">
       <c r="A188" t="s">
         <v>747</v>
       </c>
@@ -8071,7 +8104,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8">
       <c r="A189" t="s">
         <v>751</v>
       </c>
@@ -8097,7 +8130,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8">
       <c r="A190" t="s">
         <v>755</v>
       </c>
@@ -8123,7 +8156,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:8">
       <c r="A191" t="s">
         <v>759</v>
       </c>
@@ -8149,7 +8182,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:8">
       <c r="A192" t="s">
         <v>764</v>
       </c>
@@ -8175,7 +8208,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:8">
       <c r="A193" t="s">
         <v>768</v>
       </c>
@@ -8201,7 +8234,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:8">
       <c r="A194" t="s">
         <v>772</v>
       </c>
@@ -8241,27 +8274,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{818C5280-76B8-41DD-A89C-555E0F7B7960}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14:E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="31.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.5" style="2" customWidth="1"/>
-    <col min="5" max="6" width="15.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="38.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="40.5" customWidth="1"/>
+    <col min="4" max="4" width="44.44140625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="15.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="38.5546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="40.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="7" t="s">
-        <v>863</v>
+        <v>858</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>777</v>
@@ -8282,12 +8315,12 @@
         <v>778</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="84" x14ac:dyDescent="0.2">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="79.2">
       <c r="A2" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>21</v>
@@ -8298,18 +8331,22 @@
       <c r="D2" s="3" t="s">
         <v>776</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="E2" s="10">
+        <v>1</v>
+      </c>
+      <c r="F2" s="10">
+        <v>2</v>
+      </c>
       <c r="G2" s="2" t="s">
         <v>781</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="86.4">
       <c r="A3" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>44</v>
@@ -8320,16 +8357,22 @@
       <c r="D3" s="2" t="s">
         <v>784</v>
       </c>
+      <c r="E3" s="11">
+        <v>3</v>
+      </c>
+      <c r="F3" s="11">
+        <v>4</v>
+      </c>
       <c r="G3" s="2" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="187.2">
       <c r="A4" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>99</v>
@@ -8338,18 +8381,21 @@
         <v>98</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="E4" s="4">
         <v>300312096</v>
       </c>
+      <c r="F4" s="11">
+        <v>5</v>
+      </c>
       <c r="G4" s="2" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8">
       <c r="A5" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>130</v>
@@ -8360,13 +8406,19 @@
       <c r="D5" s="2" t="s">
         <v>785</v>
       </c>
+      <c r="E5" s="11">
+        <v>6</v>
+      </c>
+      <c r="F5" s="11">
+        <v>7</v>
+      </c>
       <c r="G5" s="2" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28.8">
       <c r="A6" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>133</v>
@@ -8380,13 +8432,16 @@
       <c r="E6" s="4">
         <v>300299135</v>
       </c>
+      <c r="F6" s="11">
+        <v>8</v>
+      </c>
       <c r="G6" s="2" t="s">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="27.6">
       <c r="A7" s="7" t="s">
-        <v>852</v>
+        <v>847</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>136</v>
@@ -8404,12 +8459,12 @@
         <v>788</v>
       </c>
       <c r="H7" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>227</v>
@@ -8423,13 +8478,16 @@
       <c r="E8" s="4">
         <v>300178244</v>
       </c>
+      <c r="F8" s="11">
+        <v>9</v>
+      </c>
       <c r="G8" s="2" t="s">
-        <v>853</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="86.4">
       <c r="A9" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>288</v>
@@ -8440,16 +8498,22 @@
       <c r="D9" s="2" t="s">
         <v>790</v>
       </c>
+      <c r="E9" s="11">
+        <v>10</v>
+      </c>
+      <c r="F9" s="11">
+        <v>11</v>
+      </c>
       <c r="G9" s="2" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="144">
       <c r="A10" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>291</v>
@@ -8463,13 +8527,16 @@
       <c r="E10" s="4">
         <v>300024841</v>
       </c>
+      <c r="F10" s="11">
+        <v>12</v>
+      </c>
       <c r="G10" s="5" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="43.2">
       <c r="A11" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>325</v>
@@ -8480,19 +8547,22 @@
       <c r="D11" s="2" t="s">
         <v>792</v>
       </c>
-      <c r="E11" s="4">
-        <v>300163338</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>865</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+      <c r="E11" s="12">
+        <v>13</v>
+      </c>
+      <c r="F11" s="11">
+        <v>14</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="100.8">
       <c r="A12" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>334</v>
@@ -8503,13 +8573,19 @@
       <c r="D12" s="2" t="s">
         <v>793</v>
       </c>
+      <c r="E12" s="11">
+        <v>15</v>
+      </c>
+      <c r="F12" s="11">
+        <v>16</v>
+      </c>
       <c r="G12" s="2" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>391</v>
@@ -8523,13 +8599,16 @@
       <c r="E13" s="4">
         <v>300266745</v>
       </c>
+      <c r="F13" s="11">
+        <v>17</v>
+      </c>
       <c r="G13" s="2" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="43.2">
       <c r="A14" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>422</v>
@@ -8540,16 +8619,20 @@
       <c r="D14" s="2" t="s">
         <v>795</v>
       </c>
+      <c r="E14" s="11">
+        <v>18</v>
+      </c>
+      <c r="F14" s="11"/>
       <c r="G14" s="2" t="s">
-        <v>886</v>
+        <v>880</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>882</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="72">
       <c r="A15" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>448</v>
@@ -8560,16 +8643,22 @@
       <c r="D15" s="2" t="s">
         <v>796</v>
       </c>
+      <c r="E15" s="11">
+        <v>19</v>
+      </c>
+      <c r="F15" s="11">
+        <v>20</v>
+      </c>
       <c r="G15" s="2" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="43.2">
       <c r="A16" s="7" t="s">
-        <v>852</v>
+        <v>806</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>451</v>
@@ -8578,18 +8667,21 @@
         <v>452</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="E16" s="4">
         <v>300037126</v>
       </c>
+      <c r="F16" s="11">
+        <v>21</v>
+      </c>
       <c r="G16" s="2" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="57.6">
       <c r="A17" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>463</v>
@@ -8598,18 +8690,21 @@
         <v>462</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="E17" s="2">
         <v>300198855</v>
       </c>
+      <c r="F17" s="11">
+        <v>22</v>
+      </c>
       <c r="G17" s="2" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="100.8">
       <c r="A18" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>479</v>
@@ -8623,16 +8718,19 @@
       <c r="E18" s="2">
         <v>300400908</v>
       </c>
+      <c r="F18" s="11">
+        <v>23</v>
+      </c>
       <c r="G18" s="2" t="s">
-        <v>902</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>923</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="72">
       <c r="A19" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>499</v>
@@ -8641,21 +8739,24 @@
         <v>500</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E19" s="4">
         <v>300037119</v>
       </c>
+      <c r="F19" s="11">
+        <v>24</v>
+      </c>
       <c r="G19" s="2" t="s">
-        <v>904</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+        <v>895</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="172.8">
       <c r="A20" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>561</v>
@@ -8664,21 +8765,24 @@
         <v>560</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E20" s="2">
         <v>300265725</v>
       </c>
+      <c r="F20" s="11">
+        <v>25</v>
+      </c>
       <c r="G20" s="2" t="s">
-        <v>908</v>
+        <v>898</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="57.6">
       <c r="A21" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>634</v>
@@ -8687,18 +8791,21 @@
         <v>633</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>909</v>
+        <v>899</v>
       </c>
       <c r="E21" s="2">
         <v>300198842</v>
       </c>
+      <c r="F21" s="11">
+        <v>26</v>
+      </c>
       <c r="G21" s="2" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="28.8">
       <c r="A22" s="7" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>733</v>
@@ -8709,11 +8816,14 @@
       <c r="E22" s="4">
         <v>300037110</v>
       </c>
+      <c r="F22" s="11">
+        <v>27</v>
+      </c>
       <c r="G22" s="2" t="s">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="57.6">
       <c r="B23" s="4" t="s">
         <v>745</v>
       </c>
@@ -8721,16 +8831,19 @@
         <v>744</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="E23" s="4">
         <v>300038141</v>
       </c>
+      <c r="F23" s="11">
+        <v>28</v>
+      </c>
       <c r="G23" s="2" t="s">
-        <v>804</v>
+        <v>926</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>805</v>
+        <v>922</v>
       </c>
     </row>
   </sheetData>
@@ -8786,546 +8899,630 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED727AC-8741-47CF-9019-04DDDE535DB8}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.83203125" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" customWidth="1"/>
-    <col min="7" max="7" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="73.77734375" customWidth="1"/>
+    <col min="7" max="7" width="27.21875" customWidth="1"/>
+    <col min="8" max="8" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>922</v>
-      </c>
+    <row r="1" spans="1:6">
       <c r="C1" t="s">
+        <v>909</v>
+      </c>
+      <c r="D1" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1">
+      <c r="C2" t="s">
+        <v>805</v>
+      </c>
+      <c r="D2" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1">
+      <c r="C3" t="s">
+        <v>803</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="C4" t="s">
+        <v>804</v>
+      </c>
+      <c r="D4" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" s="9" t="s">
+        <v>837</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>840</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>841</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>842</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>838</v>
+      </c>
+      <c r="C7" t="s">
         <v>815</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>809</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D7" t="s">
+        <v>813</v>
+      </c>
+      <c r="E7" t="s">
         <v>816</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>807</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="F7" t="s">
         <v>818</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>808</v>
-      </c>
-      <c r="C4" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>842</v>
-      </c>
-      <c r="B6" s="9" t="s">
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>839</v>
+      </c>
+      <c r="C8" t="s">
+        <v>815</v>
+      </c>
+      <c r="D8" t="s">
+        <v>814</v>
+      </c>
+      <c r="E8" t="s">
+        <v>820</v>
+      </c>
+      <c r="F8" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>838</v>
+      </c>
+      <c r="C9" t="s">
+        <v>822</v>
+      </c>
+      <c r="D9" t="s">
+        <v>813</v>
+      </c>
+      <c r="E9" t="s">
+        <v>821</v>
+      </c>
+      <c r="F9" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>838</v>
+      </c>
+      <c r="C10" t="s">
+        <v>822</v>
+      </c>
+      <c r="D10" t="s">
+        <v>813</v>
+      </c>
+      <c r="E10" t="s">
+        <v>824</v>
+      </c>
+      <c r="F10" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>839</v>
+      </c>
+      <c r="C11" t="s">
+        <v>826</v>
+      </c>
+      <c r="D11" t="s">
+        <v>814</v>
+      </c>
+      <c r="E11" t="s">
+        <v>827</v>
+      </c>
+      <c r="F11" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>838</v>
+      </c>
+      <c r="C12" t="s">
+        <v>831</v>
+      </c>
+      <c r="D12" t="s">
+        <v>813</v>
+      </c>
+      <c r="E12" t="s">
+        <v>830</v>
+      </c>
+      <c r="F12" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>838</v>
+      </c>
+      <c r="C13" t="s">
+        <v>831</v>
+      </c>
+      <c r="D13" t="s">
+        <v>813</v>
+      </c>
+      <c r="E13" t="s">
+        <v>833</v>
+      </c>
+      <c r="F13" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>838</v>
+      </c>
+      <c r="C14" t="s">
+        <v>843</v>
+      </c>
+      <c r="D14" t="s">
+        <v>813</v>
+      </c>
+      <c r="E14" t="s">
+        <v>844</v>
+      </c>
+      <c r="F14" t="s">
         <v>845</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>846</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>847</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>843</v>
-      </c>
-      <c r="B7" t="s">
-        <v>819</v>
-      </c>
-      <c r="C7" t="s">
-        <v>817</v>
-      </c>
-      <c r="D7" t="s">
-        <v>820</v>
-      </c>
-      <c r="E7" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>844</v>
-      </c>
-      <c r="B8" t="s">
-        <v>822</v>
-      </c>
-      <c r="C8" t="s">
-        <v>818</v>
-      </c>
-      <c r="D8" t="s">
-        <v>825</v>
-      </c>
-      <c r="E8" t="s">
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>838</v>
+      </c>
+      <c r="C15" t="s">
+        <v>849</v>
+      </c>
+      <c r="D15" t="s">
+        <v>813</v>
+      </c>
+      <c r="E15" t="s">
+        <v>850</v>
+      </c>
+      <c r="F15" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>839</v>
+      </c>
+      <c r="C16" t="s">
+        <v>853</v>
+      </c>
+      <c r="D16" t="s">
+        <v>814</v>
+      </c>
+      <c r="E16" t="s">
+        <v>856</v>
+      </c>
+      <c r="F16" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>839</v>
+      </c>
+      <c r="C17" t="s">
+        <v>853</v>
+      </c>
+      <c r="D17" t="s">
+        <v>814</v>
+      </c>
+      <c r="E17" t="s">
+        <v>854</v>
+      </c>
+      <c r="F17" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>838</v>
+      </c>
+      <c r="C18" t="s">
+        <v>910</v>
+      </c>
+      <c r="D18" t="s">
+        <v>813</v>
+      </c>
+      <c r="E18" t="s">
+        <v>914</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>862</v>
+      </c>
+      <c r="C19" t="s">
+        <v>861</v>
+      </c>
+      <c r="D19" t="s">
+        <v>812</v>
+      </c>
+      <c r="E19" t="s">
+        <v>863</v>
+      </c>
+      <c r="F19" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>862</v>
+      </c>
+      <c r="C20" t="s">
+        <v>861</v>
+      </c>
+      <c r="D20" t="s">
+        <v>812</v>
+      </c>
+      <c r="E20" t="s">
+        <v>866</v>
+      </c>
+      <c r="F20" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>838</v>
+      </c>
+      <c r="C21" t="s">
+        <v>867</v>
+      </c>
+      <c r="D21" t="s">
+        <v>813</v>
+      </c>
+      <c r="E21" t="s">
+        <v>870</v>
+      </c>
+      <c r="F21" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>838</v>
+      </c>
+      <c r="C22" t="s">
+        <v>867</v>
+      </c>
+      <c r="D22" t="s">
+        <v>813</v>
+      </c>
+      <c r="E22" t="s">
+        <v>868</v>
+      </c>
+      <c r="F22" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>838</v>
+      </c>
+      <c r="C23" t="s">
+        <v>911</v>
+      </c>
+      <c r="D23" t="s">
+        <v>813</v>
+      </c>
+      <c r="E23" t="s">
+        <v>873</v>
+      </c>
+      <c r="F23" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>838</v>
+      </c>
+      <c r="C24" t="s">
+        <v>878</v>
+      </c>
+      <c r="D24" t="s">
+        <v>813</v>
+      </c>
+      <c r="E24" t="s">
+        <v>877</v>
+      </c>
+      <c r="F24" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>839</v>
+      </c>
+      <c r="C25" t="s">
+        <v>881</v>
+      </c>
+      <c r="D25" t="s">
+        <v>814</v>
+      </c>
+      <c r="E25" t="s">
+        <v>882</v>
+      </c>
+      <c r="F25" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>838</v>
+      </c>
+      <c r="C26" t="s">
+        <v>881</v>
+      </c>
+      <c r="D26" t="s">
+        <v>813</v>
+      </c>
+      <c r="E26" t="s">
+        <v>884</v>
+      </c>
+      <c r="F26" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>838</v>
+      </c>
+      <c r="C27" t="s">
+        <v>917</v>
+      </c>
+      <c r="D27" t="s">
+        <v>813</v>
+      </c>
+      <c r="E27" t="s">
         <v>824</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>843</v>
-      </c>
-      <c r="B9" t="s">
-        <v>827</v>
-      </c>
-      <c r="C9" t="s">
-        <v>817</v>
-      </c>
-      <c r="D9" t="s">
-        <v>826</v>
-      </c>
-      <c r="E9" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>843</v>
-      </c>
-      <c r="B10" t="s">
-        <v>827</v>
-      </c>
-      <c r="C10" t="s">
-        <v>817</v>
-      </c>
-      <c r="D10" t="s">
-        <v>829</v>
-      </c>
-      <c r="E10" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>844</v>
-      </c>
-      <c r="B11" t="s">
-        <v>831</v>
-      </c>
-      <c r="C11" t="s">
-        <v>818</v>
-      </c>
-      <c r="D11" t="s">
-        <v>832</v>
-      </c>
-      <c r="E11" t="s">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>843</v>
-      </c>
-      <c r="B12" t="s">
-        <v>836</v>
-      </c>
-      <c r="C12" t="s">
-        <v>817</v>
-      </c>
-      <c r="D12" t="s">
-        <v>835</v>
-      </c>
-      <c r="E12" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>843</v>
-      </c>
-      <c r="B13" t="s">
-        <v>836</v>
-      </c>
-      <c r="C13" t="s">
-        <v>817</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="F27" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
         <v>838</v>
       </c>
-      <c r="E13" t="s">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>843</v>
-      </c>
-      <c r="B14" t="s">
-        <v>848</v>
-      </c>
-      <c r="C14" t="s">
-        <v>817</v>
-      </c>
-      <c r="D14" t="s">
-        <v>849</v>
-      </c>
-      <c r="E14" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>843</v>
-      </c>
-      <c r="B15" t="s">
-        <v>854</v>
-      </c>
-      <c r="C15" t="s">
-        <v>817</v>
-      </c>
-      <c r="D15" t="s">
-        <v>855</v>
-      </c>
-      <c r="E15" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>844</v>
-      </c>
-      <c r="B16" t="s">
-        <v>858</v>
-      </c>
-      <c r="C16" t="s">
-        <v>818</v>
-      </c>
-      <c r="D16" t="s">
-        <v>859</v>
-      </c>
-      <c r="E16" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>844</v>
-      </c>
-      <c r="B17" t="s">
-        <v>858</v>
-      </c>
-      <c r="C17" t="s">
-        <v>818</v>
-      </c>
-      <c r="D17" t="s">
-        <v>861</v>
-      </c>
-      <c r="E17" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>867</v>
-      </c>
-      <c r="B18" t="s">
-        <v>866</v>
-      </c>
-      <c r="C18" t="s">
-        <v>816</v>
-      </c>
-      <c r="D18" t="s">
-        <v>868</v>
-      </c>
-      <c r="E18" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>867</v>
-      </c>
-      <c r="B19" t="s">
-        <v>866</v>
-      </c>
-      <c r="C19" t="s">
-        <v>816</v>
-      </c>
-      <c r="D19" t="s">
-        <v>871</v>
-      </c>
-      <c r="E19" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>843</v>
-      </c>
-      <c r="B20" t="s">
-        <v>872</v>
-      </c>
-      <c r="C20" t="s">
-        <v>817</v>
-      </c>
-      <c r="D20" t="s">
-        <v>876</v>
-      </c>
-      <c r="E20" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>843</v>
-      </c>
-      <c r="B21" t="s">
-        <v>872</v>
-      </c>
-      <c r="C21" t="s">
-        <v>817</v>
-      </c>
-      <c r="D21" t="s">
-        <v>873</v>
-      </c>
-      <c r="E21" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>843</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="C28" t="s">
+        <v>891</v>
+      </c>
+      <c r="D28" t="s">
+        <v>813</v>
+      </c>
+      <c r="E28" t="s">
+        <v>892</v>
+      </c>
+      <c r="F28" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>23</v>
+      </c>
+      <c r="B29" t="s">
+        <v>838</v>
+      </c>
+      <c r="C29" t="s">
+        <v>894</v>
+      </c>
+      <c r="D29" t="s">
+        <v>813</v>
+      </c>
+      <c r="E29" t="s">
         <v>924</v>
       </c>
-      <c r="C22" t="s">
-        <v>817</v>
-      </c>
-      <c r="D22" t="s">
-        <v>879</v>
-      </c>
-      <c r="E22" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>843</v>
-      </c>
-      <c r="B23" t="s">
-        <v>884</v>
-      </c>
-      <c r="C23" t="s">
-        <v>817</v>
-      </c>
-      <c r="D23" t="s">
-        <v>883</v>
-      </c>
-      <c r="E23" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>844</v>
-      </c>
-      <c r="B24" t="s">
-        <v>887</v>
-      </c>
-      <c r="C24" t="s">
-        <v>818</v>
-      </c>
-      <c r="D24" t="s">
-        <v>888</v>
-      </c>
-      <c r="E24" t="s">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>843</v>
-      </c>
-      <c r="B25" t="s">
-        <v>887</v>
-      </c>
-      <c r="C25" t="s">
-        <v>817</v>
-      </c>
-      <c r="D25" t="s">
-        <v>890</v>
-      </c>
-      <c r="E25" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>843</v>
-      </c>
-      <c r="B26" t="s">
-        <v>898</v>
-      </c>
-      <c r="C26" t="s">
-        <v>817</v>
-      </c>
-      <c r="D26" t="s">
-        <v>899</v>
-      </c>
-      <c r="E26" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>843</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="F29" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s">
+        <v>838</v>
+      </c>
+      <c r="C30" t="s">
+        <v>896</v>
+      </c>
+      <c r="D30" t="s">
+        <v>813</v>
+      </c>
+      <c r="E30" t="s">
+        <v>824</v>
+      </c>
+      <c r="F30" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>25</v>
+      </c>
+      <c r="B31" t="s">
+        <v>838</v>
+      </c>
+      <c r="C31" t="s">
+        <v>912</v>
+      </c>
+      <c r="D31" t="s">
+        <v>813</v>
+      </c>
+      <c r="E31" t="s">
+        <v>913</v>
+      </c>
+      <c r="F31" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>838</v>
+      </c>
+      <c r="C32" t="s">
+        <v>901</v>
+      </c>
+      <c r="D32" t="s">
+        <v>813</v>
+      </c>
+      <c r="E32" t="s">
+        <v>902</v>
+      </c>
+      <c r="F32" t="s">
         <v>903</v>
       </c>
-      <c r="C27" t="s">
-        <v>817</v>
-      </c>
-      <c r="D27" t="s">
-        <v>901</v>
-      </c>
-      <c r="E27" t="s">
+    </row>
+    <row r="33" spans="1:6" ht="16.8" customHeight="1">
+      <c r="A33">
+        <v>27</v>
+      </c>
+      <c r="B33" t="s">
+        <v>838</v>
+      </c>
+      <c r="C33" t="s">
+        <v>904</v>
+      </c>
+      <c r="D33" t="s">
+        <v>813</v>
+      </c>
+      <c r="E33" t="s">
+        <v>824</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>28</v>
+      </c>
+      <c r="B34" t="s">
+        <v>838</v>
+      </c>
+      <c r="C34" t="s">
+        <v>906</v>
+      </c>
+      <c r="D34" t="s">
+        <v>813</v>
+      </c>
+      <c r="E34" t="s">
         <v>907</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>843</v>
-      </c>
-      <c r="B28" t="s">
-        <v>905</v>
-      </c>
-      <c r="C28" t="s">
-        <v>817</v>
-      </c>
-      <c r="D28" t="s">
-        <v>829</v>
-      </c>
-      <c r="E28" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>843</v>
-      </c>
-      <c r="B29" t="s">
-        <v>925</v>
-      </c>
-      <c r="C29" t="s">
-        <v>817</v>
-      </c>
-      <c r="D29" t="s">
-        <v>926</v>
-      </c>
-      <c r="E29" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>843</v>
-      </c>
-      <c r="B30" t="s">
-        <v>911</v>
-      </c>
-      <c r="C30" t="s">
-        <v>817</v>
-      </c>
-      <c r="D30" t="s">
-        <v>912</v>
-      </c>
-      <c r="E30" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>843</v>
-      </c>
-      <c r="B31" t="s">
-        <v>915</v>
-      </c>
-      <c r="C31" t="s">
-        <v>817</v>
-      </c>
-      <c r="D31" t="s">
-        <v>829</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>843</v>
-      </c>
-      <c r="B32" t="s">
-        <v>917</v>
-      </c>
-      <c r="C32" t="s">
-        <v>817</v>
-      </c>
-      <c r="D32" t="s">
-        <v>918</v>
-      </c>
-      <c r="E32" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>843</v>
-      </c>
-      <c r="B33" t="s">
-        <v>917</v>
-      </c>
-      <c r="C33" t="s">
-        <v>817</v>
-      </c>
-      <c r="D33" t="s">
-        <v>920</v>
-      </c>
-      <c r="E33" t="s">
-        <v>921</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>843</v>
-      </c>
-      <c r="B34" t="s">
-        <v>923</v>
-      </c>
-      <c r="C34" t="s">
-        <v>817</v>
-      </c>
-      <c r="D34" t="s">
-        <v>927</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>928</v>
+      <c r="F34" t="s">
+        <v>908</v>
       </c>
     </row>
   </sheetData>

</xml_diff>